<commit_message>
File con modifiche ai test 32 e 40
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#EBNEUROSPAXX/EBNeuro/Galileo/4.60/report-checklist.xlsx
+++ b/GATEWAY/A1#111#EBNEUROSPAXX/EBNeuro/Galileo/4.60/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpratesi\Desktop\FSE\EBNeuro\EBNeuro\Galileo\4.60\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpratesi\Desktop\A1#111#EBNEUROSPAXX\EBNeuro\Galileo\4.60\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB109414-CDF3-424A-A753-6286D39999D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DC82B6-987B-4BF6-A327-C75B69A08972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="219">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -879,33 +879,6 @@
     <t>Nel nostro applicativo gli unici campi che possono essere estratti in modo strutturato sono quelli obbligatori, ossia il testo del referto e le prestazioni eseguite, non esistono campi strutturati per descrivere le procedure eseguite e/o relative analisi, qualcosa è possibile ricavare ma solo come testo libero non strutturato.</t>
   </si>
   <si>
-    <t>2024-10-07T14:09:00Z</t>
-  </si>
-  <si>
-    <t>xxx</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.LOCAL1483638639139840515123LOCAL314811134^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>ERROR: Per maggiori dettagli vedere i logs applicativi 403 Il codice fiscale nel campo sub non è corretto [/msg/jwt-validation]</t>
-  </si>
-  <si>
-    <t>2024-10-07T13:55:00Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.LOCAL1463638639130673191946LOCAL314611132^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERROR: Per maggiori dettagli vedere i logs applicativi 401 Required token claims not found </t>
-  </si>
-  <si>
-    <t>Come facciamo a generare un timeout? Avete degli url da chiamare che lo simulano?</t>
-  </si>
-  <si>
-    <t>Per generare un timeout dobbiamo chiamare un url che esiste ma che non risponde in tempo, in alternativa possiamo generare un errore simulandolo ma non sarebbe diverso da ogni altro errore per il nostro sistema, sarebbe un errore mostrato all'utente che dovrebbe ritentare dopo alche secondo oppure avvisare il service se l'errore persiste.</t>
-  </si>
-  <si>
     <t>Questo tipo di errore genera un messaggio a video al medico, in questo scenario deve per forza intervenire il nostro service, una volta risolto il problema, il medico dovrà ripetere la procedura per completare il cilco di lavoro. Il nostro flusso di lavoro prevede che la procedura di "Firma Referto e Marca Completato" sia eseguita al termine del lavoro, pertanto un errore in questa procedura non impedisce al medico di completare l'esame, non influisce sull'esperienza del paziente in ambulatorio, il medico potrà completare la procedura in qualsiasi momento dopo la risoluzione del problema.</t>
   </si>
   <si>
@@ -916,6 +889,27 @@
   </si>
   <si>
     <t>Come pe tutti gli altri errori, il medico riceve un messaggio a video con alcuni dettagli dell'errore, ma in questo scenario lui non può risolvere la situazione, deve contattare il nostro service, al termine delle operazioni di ripristino il medico deve necessariamente ripetere la procedura di firma del referto, ma essendo in pratica l'ultima procedura prima di considerare l'esame completo non è bloccante ai fini del lavoro.</t>
+  </si>
+  <si>
+    <t>ERROR:Campo token JWT non valido.,Il campo action_id non è corretto.</t>
+  </si>
+  <si>
+    <t>ERROR:Timeout dai servizi centrali.</t>
+  </si>
+  <si>
+    <t>ERROR:Campo token JWT non valido, Il campo purpose_of_use non è valorizzato.</t>
+  </si>
+  <si>
+    <t>fb074ad567960800</t>
+  </si>
+  <si>
+    <t>2024-11-27T07:50:00Z</t>
+  </si>
+  <si>
+    <t>98183e706775abb4</t>
+  </si>
+  <si>
+    <t>2024-11-27T08:09:00Z</t>
   </si>
 </sst>
 </file>
@@ -1037,7 +1031,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1064,8 +1058,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB8E08C"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -1441,7 +1441,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1518,33 +1518,6 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1583,6 +1556,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3056,10 +3032,10 @@
   <dimension ref="A1:W620"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3103,14 +3079,14 @@
       <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="D2" s="57"/>
+      <c r="D2" s="49"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
@@ -3131,14 +3107,14 @@
       <c r="W2" s="9"/>
     </row>
     <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="60"/>
-      <c r="C3" s="65" t="s">
+      <c r="B3" s="52"/>
+      <c r="C3" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="D3" s="57"/>
+      <c r="D3" s="49"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
@@ -3159,12 +3135,12 @@
       <c r="W3" s="9"/>
     </row>
     <row r="4" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="65" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="57"/>
+      <c r="D4" s="49"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
@@ -3186,12 +3162,12 @@
       <c r="W4" s="9"/>
     </row>
     <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="63"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="65" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="D5" s="57"/>
+      <c r="D5" s="49"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
@@ -3212,8 +3188,8 @@
       <c r="W5" s="9"/>
     </row>
     <row r="6" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="10"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -3311,7 +3287,7 @@
       <c r="K9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="L9" s="45" t="s">
         <v>101</v>
       </c>
       <c r="M9" s="20" t="s">
@@ -3348,1450 +3324,1438 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30">
+    <row r="10" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="34">
         <v>32</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="37">
+        <v>45623</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="H10" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N10" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" s="39" t="s">
+        <v>214</v>
+      </c>
+      <c r="P10" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q10" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R10" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S10" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="T10" s="39"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="34">
+        <v>40</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="37">
+        <v>45623</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="H11" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="39"/>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N11" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" s="39" t="s">
+        <v>212</v>
+      </c>
+      <c r="P11" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q11" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R11" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S11" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="T11" s="39"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34">
+        <v>48</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
+      <c r="M12" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="P12" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q12" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R12" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S12" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="T12" s="39"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="34">
+        <v>147</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="W13" s="42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="34">
+        <v>148</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="F14" s="37"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K14" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="W14" s="42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="34">
+        <v>149</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K15" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="W15" s="42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34">
+        <v>150</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="W16" s="42" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34">
+        <v>151</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="37">
+        <v>45566</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="H17" s="38" t="s">
+        <v>199</v>
+      </c>
+      <c r="I17" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="J17" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K17" s="39"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="P17" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q17" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R17" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S17" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="T17" s="39"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W17" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="34">
+        <v>152</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="F18" s="37">
+        <v>45566.70208333333</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>196</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="J18" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N18" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O18" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="P18" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q18" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R18" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S18" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="T18" s="39"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W18" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34">
+        <v>153</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="37">
+        <v>45569</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="H19" s="38" t="s">
+        <v>194</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="J19" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N19" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O19" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="P19" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q19" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R19" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S19" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="T19" s="39"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W19" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34">
+        <v>154</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" s="37">
+        <v>45569</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="H20" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="I20" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="J20" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N20" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O20" s="39" t="s">
+        <v>154</v>
+      </c>
+      <c r="P20" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q20" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R20" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S20" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="T20" s="39"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W20" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="34">
+        <v>155</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="37">
+        <v>45569</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="H21" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>189</v>
+      </c>
+      <c r="J21" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N21" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O21" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="P21" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q21" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R21" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S21" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="T21" s="39"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W21" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="34">
+        <v>156</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="36" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="37">
+        <v>45569</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="H22" s="38" t="s">
+        <v>185</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="J22" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N22" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O22" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="P22" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q22" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R22" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S22" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="T22" s="39"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W22" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="34">
+        <v>157</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K23" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39"/>
+      <c r="N23" s="39"/>
+      <c r="O23" s="39"/>
+      <c r="P23" s="39"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="41"/>
+      <c r="W23" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="34">
+        <v>158</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="F24" s="37">
         <v>45572</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="I10" s="34" t="s">
+      <c r="G24" s="38" t="s">
+        <v>180</v>
+      </c>
+      <c r="H24" s="38" t="s">
+        <v>181</v>
+      </c>
+      <c r="I24" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="J24" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N24" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O24" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="P24" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q24" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R24" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S24" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="T24" s="39"/>
+      <c r="U24" s="40"/>
+      <c r="V24" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W24" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="34">
+        <v>159</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" s="37">
+        <v>45572</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="H25" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="I25" s="38" t="s">
+        <v>179</v>
+      </c>
+      <c r="J25" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N25" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O25" s="39" t="s">
+        <v>159</v>
+      </c>
+      <c r="P25" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q25" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R25" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S25" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="T25" s="39"/>
+      <c r="U25" s="40"/>
+      <c r="V25" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W25" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="34">
+        <v>160</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="37">
+        <v>45572</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="H26" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="I26" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="J26" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N26" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O26" s="39" t="s">
+        <v>160</v>
+      </c>
+      <c r="P26" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q26" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R26" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S26" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="T26" s="39"/>
+      <c r="U26" s="40"/>
+      <c r="V26" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W26" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="34">
+        <v>161</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F27" s="37">
+        <v>45572</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="H27" s="38" t="s">
+        <v>164</v>
+      </c>
+      <c r="I27" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="J27" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N27" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O27" s="39" t="s">
+        <v>166</v>
+      </c>
+      <c r="P27" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q27" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R27" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S27" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="T27" s="39"/>
+      <c r="U27" s="40"/>
+      <c r="V27" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W27" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="34">
+        <v>162</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K28" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="39"/>
+      <c r="T28" s="39"/>
+      <c r="U28" s="40"/>
+      <c r="V28" s="41"/>
+      <c r="W28" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="34">
+        <v>163</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="37">
+        <v>45572</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="H29" s="38" t="s">
+        <v>171</v>
+      </c>
+      <c r="I29" s="38" t="s">
+        <v>172</v>
+      </c>
+      <c r="J29" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35" t="s">
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="N10" s="35" t="s">
+      <c r="N29" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="O10" s="35" t="s">
+      <c r="O29" s="39" t="s">
+        <v>173</v>
+      </c>
+      <c r="P29" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q29" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R29" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S29" s="39" t="s">
+        <v>210</v>
+      </c>
+      <c r="T29" s="39"/>
+      <c r="U29" s="40"/>
+      <c r="V29" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="W29" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="34">
+        <v>164</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K30" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="39"/>
+      <c r="Q30" s="39"/>
+      <c r="R30" s="39"/>
+      <c r="S30" s="39"/>
+      <c r="T30" s="39"/>
+      <c r="U30" s="40"/>
+      <c r="V30" s="41"/>
+      <c r="W30" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34">
+        <v>165</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="F31" s="37"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K31" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="39"/>
+      <c r="Q31" s="39"/>
+      <c r="R31" s="39"/>
+      <c r="S31" s="39"/>
+      <c r="T31" s="39"/>
+      <c r="U31" s="40"/>
+      <c r="V31" s="41"/>
+      <c r="W31" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="34">
+        <v>166</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="F32" s="37"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K32" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="39"/>
+      <c r="S32" s="39"/>
+      <c r="T32" s="39"/>
+      <c r="U32" s="40"/>
+      <c r="V32" s="41"/>
+      <c r="W32" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="34">
+        <v>167</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E33" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="F33" s="37"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K33" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="39"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="39"/>
+      <c r="R33" s="39"/>
+      <c r="S33" s="39"/>
+      <c r="T33" s="39"/>
+      <c r="U33" s="40"/>
+      <c r="V33" s="41"/>
+      <c r="W33" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="34">
+        <v>168</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="F34" s="37"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="K34" s="39" t="s">
+        <v>105</v>
+      </c>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="39"/>
+      <c r="Q34" s="39"/>
+      <c r="R34" s="39"/>
+      <c r="S34" s="39"/>
+      <c r="T34" s="39"/>
+      <c r="U34" s="40"/>
+      <c r="V34" s="41"/>
+      <c r="W34" s="42" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="34">
+        <v>169</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" s="37">
+        <v>45572</v>
+      </c>
+      <c r="G35" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="H35" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="I35" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="J35" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="N35" s="39" t="s">
+        <v>49</v>
+      </c>
+      <c r="O35" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="P35" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q35" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="R35" s="39" t="s">
+        <v>100</v>
+      </c>
+      <c r="S35" s="39" t="s">
         <v>211</v>
       </c>
-      <c r="P10" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q10" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R10" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S10" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="T10" s="35"/>
-      <c r="U10" s="36"/>
-      <c r="V10" s="37" t="s">
+      <c r="T35" s="39"/>
+      <c r="U35" s="40"/>
+      <c r="V35" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="W10" s="38" t="s">
+      <c r="W35" s="42" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30">
-        <v>40</v>
-      </c>
-      <c r="B11" s="31" t="s">
+    <row r="36" spans="1:23" s="43" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="34">
+        <v>374</v>
+      </c>
+      <c r="B36" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C36" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="33">
+      <c r="D36" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="F36" s="37">
         <v>45572</v>
       </c>
-      <c r="G11" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="J11" s="35" t="s">
+      <c r="G36" s="38" t="s">
+        <v>201</v>
+      </c>
+      <c r="H36" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="I36" s="38" t="s">
+        <v>203</v>
+      </c>
+      <c r="J36" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N11" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O11" s="35" t="s">
-        <v>214</v>
-      </c>
-      <c r="P11" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q11" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R11" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S11" s="35" t="s">
-        <v>217</v>
-      </c>
-      <c r="T11" s="35"/>
-      <c r="U11" s="36"/>
-      <c r="V11" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W11" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30">
-        <v>48</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K12" s="35" t="s">
-        <v>111</v>
-      </c>
-      <c r="L12" s="35" t="s">
-        <v>215</v>
-      </c>
-      <c r="M12" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N12" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q12" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R12" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S12" s="35" t="s">
-        <v>218</v>
-      </c>
-      <c r="T12" s="35"/>
-      <c r="U12" s="36"/>
-      <c r="V12" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="W12" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" s="52" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="43">
-        <v>147</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="F13" s="46"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="47"/>
-      <c r="J13" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="K13" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="L13" s="48"/>
-      <c r="M13" s="48"/>
-      <c r="N13" s="48"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="48"/>
-      <c r="R13" s="48"/>
-      <c r="S13" s="48"/>
-      <c r="T13" s="48"/>
-      <c r="U13" s="49"/>
-      <c r="V13" s="50" t="s">
-        <v>207</v>
-      </c>
-      <c r="W13" s="51" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" s="52" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="43">
-        <v>148</v>
-      </c>
-      <c r="B14" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="47"/>
-      <c r="J14" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="K14" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="L14" s="48"/>
-      <c r="M14" s="48"/>
-      <c r="N14" s="48"/>
-      <c r="O14" s="48"/>
-      <c r="P14" s="48"/>
-      <c r="Q14" s="48"/>
-      <c r="R14" s="48"/>
-      <c r="S14" s="48"/>
-      <c r="T14" s="48"/>
-      <c r="U14" s="49"/>
-      <c r="V14" s="50" t="s">
-        <v>205</v>
-      </c>
-      <c r="W14" s="51" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" s="52" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="43">
-        <v>149</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="K15" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="L15" s="48"/>
-      <c r="M15" s="48"/>
-      <c r="N15" s="48"/>
-      <c r="O15" s="48"/>
-      <c r="P15" s="48"/>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="48"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="48"/>
-      <c r="U15" s="49"/>
-      <c r="V15" s="50" t="s">
-        <v>206</v>
-      </c>
-      <c r="W15" s="51" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" s="52" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43">
-        <v>150</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="45" t="s">
-        <v>138</v>
-      </c>
-      <c r="F16" s="46"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="K16" s="48" t="s">
-        <v>105</v>
-      </c>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="48"/>
-      <c r="R16" s="48"/>
-      <c r="S16" s="48"/>
-      <c r="T16" s="48"/>
-      <c r="U16" s="49"/>
-      <c r="V16" s="50" t="s">
-        <v>206</v>
-      </c>
-      <c r="W16" s="51" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30">
-        <v>151</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="33">
-        <v>45566</v>
-      </c>
-      <c r="G17" s="34" t="s">
-        <v>198</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>199</v>
-      </c>
-      <c r="I17" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="J17" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N17" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O17" s="35" t="s">
-        <v>151</v>
-      </c>
-      <c r="P17" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q17" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R17" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S17" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="T17" s="35"/>
-      <c r="U17" s="36"/>
-      <c r="V17" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W17" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30">
-        <v>152</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>139</v>
-      </c>
-      <c r="F18" s="33">
-        <v>45566.70208333333</v>
-      </c>
-      <c r="G18" s="34" t="s">
-        <v>196</v>
-      </c>
-      <c r="H18" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="I18" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="J18" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N18" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O18" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="P18" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q18" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R18" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S18" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="T18" s="35"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W18" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30">
-        <v>153</v>
-      </c>
-      <c r="B19" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="F19" s="33">
-        <v>45569</v>
-      </c>
-      <c r="G19" s="34" t="s">
-        <v>193</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>194</v>
-      </c>
-      <c r="I19" s="34" t="s">
-        <v>195</v>
-      </c>
-      <c r="J19" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N19" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O19" s="35" t="s">
-        <v>153</v>
-      </c>
-      <c r="P19" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q19" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R19" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S19" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="T19" s="35"/>
-      <c r="U19" s="36"/>
-      <c r="V19" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W19" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30">
-        <v>154</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="F20" s="33">
-        <v>45569</v>
-      </c>
-      <c r="G20" s="34" t="s">
-        <v>190</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>191</v>
-      </c>
-      <c r="I20" s="34" t="s">
-        <v>192</v>
-      </c>
-      <c r="J20" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N20" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O20" s="35" t="s">
-        <v>154</v>
-      </c>
-      <c r="P20" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q20" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R20" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S20" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="T20" s="35"/>
-      <c r="U20" s="36"/>
-      <c r="V20" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W20" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="30">
-        <v>155</v>
-      </c>
-      <c r="B21" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="F21" s="33">
-        <v>45569</v>
-      </c>
-      <c r="G21" s="34" t="s">
-        <v>187</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>188</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>189</v>
-      </c>
-      <c r="J21" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N21" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O21" s="35" t="s">
-        <v>155</v>
-      </c>
-      <c r="P21" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q21" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R21" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S21" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="T21" s="35"/>
-      <c r="U21" s="36"/>
-      <c r="V21" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W21" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30">
-        <v>156</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="F22" s="33">
-        <v>45569</v>
-      </c>
-      <c r="G22" s="34" t="s">
-        <v>184</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>185</v>
-      </c>
-      <c r="I22" s="34" t="s">
-        <v>186</v>
-      </c>
-      <c r="J22" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N22" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O22" s="35" t="s">
-        <v>156</v>
-      </c>
-      <c r="P22" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q22" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R22" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S22" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="T22" s="35"/>
-      <c r="U22" s="36"/>
-      <c r="V22" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W22" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="30">
-        <v>157</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>144</v>
-      </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K23" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="36"/>
-      <c r="V23" s="37"/>
-      <c r="W23" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="30">
-        <v>158</v>
-      </c>
-      <c r="B24" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="F24" s="33">
-        <v>45572</v>
-      </c>
-      <c r="G24" s="34" t="s">
-        <v>180</v>
-      </c>
-      <c r="H24" s="34" t="s">
-        <v>181</v>
-      </c>
-      <c r="I24" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="J24" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N24" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O24" s="35" t="s">
-        <v>158</v>
-      </c>
-      <c r="P24" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q24" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R24" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S24" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="T24" s="35"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W24" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="30">
-        <v>159</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="33">
-        <v>45572</v>
-      </c>
-      <c r="G25" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="H25" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="I25" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="J25" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N25" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O25" s="35" t="s">
-        <v>159</v>
-      </c>
-      <c r="P25" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q25" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R25" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S25" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="T25" s="35"/>
-      <c r="U25" s="36"/>
-      <c r="V25" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W25" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="30">
-        <v>160</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="33">
-        <v>45572</v>
-      </c>
-      <c r="G26" s="34" t="s">
-        <v>167</v>
-      </c>
-      <c r="H26" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="I26" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="J26" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K26" s="35"/>
-      <c r="L26" s="35"/>
-      <c r="M26" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N26" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O26" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="P26" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q26" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R26" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S26" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="T26" s="35"/>
-      <c r="U26" s="36"/>
-      <c r="V26" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W26" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="30">
-        <v>161</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="32" t="s">
-        <v>126</v>
-      </c>
-      <c r="F27" s="33">
-        <v>45572</v>
-      </c>
-      <c r="G27" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="H27" s="34" t="s">
-        <v>164</v>
-      </c>
-      <c r="I27" s="34" t="s">
-        <v>165</v>
-      </c>
-      <c r="J27" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-      <c r="M27" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N27" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O27" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="P27" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q27" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R27" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S27" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="T27" s="35"/>
-      <c r="U27" s="36"/>
-      <c r="V27" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W27" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30">
-        <v>162</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D28" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="F28" s="33"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K28" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="L28" s="35"/>
-      <c r="M28" s="35"/>
-      <c r="N28" s="35"/>
-      <c r="O28" s="35"/>
-      <c r="P28" s="35"/>
-      <c r="Q28" s="35"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="35"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="36"/>
-      <c r="V28" s="37"/>
-      <c r="W28" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="30">
-        <v>163</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="F29" s="33">
-        <v>45572</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="H29" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="I29" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="J29" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K29" s="35"/>
-      <c r="L29" s="35"/>
-      <c r="M29" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N29" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O29" s="35" t="s">
-        <v>173</v>
-      </c>
-      <c r="P29" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q29" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R29" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S29" s="35" t="s">
-        <v>219</v>
-      </c>
-      <c r="T29" s="35"/>
-      <c r="U29" s="36"/>
-      <c r="V29" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W29" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="30">
-        <v>164</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D30" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="F30" s="33"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-      <c r="J30" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K30" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="L30" s="35"/>
-      <c r="M30" s="35"/>
-      <c r="N30" s="35"/>
-      <c r="O30" s="35"/>
-      <c r="P30" s="35"/>
-      <c r="Q30" s="35"/>
-      <c r="R30" s="35"/>
-      <c r="S30" s="35"/>
-      <c r="T30" s="35"/>
-      <c r="U30" s="36"/>
-      <c r="V30" s="37"/>
-      <c r="W30" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="30">
-        <v>165</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>130</v>
-      </c>
-      <c r="F31" s="33"/>
-      <c r="G31" s="34"/>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K31" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="35"/>
-      <c r="O31" s="35"/>
-      <c r="P31" s="35"/>
-      <c r="Q31" s="35"/>
-      <c r="R31" s="35"/>
-      <c r="S31" s="35"/>
-      <c r="T31" s="35"/>
-      <c r="U31" s="36"/>
-      <c r="V31" s="37"/>
-      <c r="W31" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="30">
-        <v>166</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>131</v>
-      </c>
-      <c r="F32" s="33"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K32" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
-      <c r="O32" s="35"/>
-      <c r="P32" s="35"/>
-      <c r="Q32" s="35"/>
-      <c r="R32" s="35"/>
-      <c r="S32" s="35"/>
-      <c r="T32" s="35"/>
-      <c r="U32" s="36"/>
-      <c r="V32" s="37"/>
-      <c r="W32" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="30">
-        <v>167</v>
-      </c>
-      <c r="B33" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D33" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K33" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="35"/>
-      <c r="O33" s="35"/>
-      <c r="P33" s="35"/>
-      <c r="Q33" s="35"/>
-      <c r="R33" s="35"/>
-      <c r="S33" s="35"/>
-      <c r="T33" s="35"/>
-      <c r="U33" s="36"/>
-      <c r="V33" s="37"/>
-      <c r="W33" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="30">
-        <v>168</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="F34" s="33"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="K34" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="L34" s="35"/>
-      <c r="M34" s="35"/>
-      <c r="N34" s="35"/>
-      <c r="O34" s="35"/>
-      <c r="P34" s="35"/>
-      <c r="Q34" s="35"/>
-      <c r="R34" s="35"/>
-      <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="36"/>
-      <c r="V34" s="37"/>
-      <c r="W34" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:23" s="39" customFormat="1" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="30">
-        <v>169</v>
-      </c>
-      <c r="B35" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="E35" s="32" t="s">
-        <v>134</v>
-      </c>
-      <c r="F35" s="33">
-        <v>45572</v>
-      </c>
-      <c r="G35" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="H35" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="I35" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="J35" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K35" s="35"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="N35" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="O35" s="35" t="s">
-        <v>162</v>
-      </c>
-      <c r="P35" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q35" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="R35" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="S35" s="35" t="s">
-        <v>220</v>
-      </c>
-      <c r="T35" s="35"/>
-      <c r="U35" s="36"/>
-      <c r="V35" s="37" t="s">
-        <v>157</v>
-      </c>
-      <c r="W35" s="38" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" s="52" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="43">
-        <v>374</v>
-      </c>
-      <c r="B36" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D36" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="F36" s="46">
-        <v>45572</v>
-      </c>
-      <c r="G36" s="47" t="s">
-        <v>201</v>
-      </c>
-      <c r="H36" s="47" t="s">
-        <v>202</v>
-      </c>
-      <c r="I36" s="47" t="s">
-        <v>203</v>
-      </c>
-      <c r="J36" s="48" t="s">
-        <v>49</v>
-      </c>
-      <c r="K36" s="48"/>
-      <c r="L36" s="48"/>
-      <c r="M36" s="48"/>
-      <c r="N36" s="48"/>
-      <c r="O36" s="48"/>
-      <c r="P36" s="48"/>
-      <c r="Q36" s="48"/>
-      <c r="R36" s="48"/>
-      <c r="S36" s="48"/>
-      <c r="T36" s="48"/>
-      <c r="U36" s="49"/>
-      <c r="V36" s="50" t="s">
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39"/>
+      <c r="P36" s="39"/>
+      <c r="Q36" s="39"/>
+      <c r="R36" s="39"/>
+      <c r="S36" s="39"/>
+      <c r="T36" s="39"/>
+      <c r="U36" s="40"/>
+      <c r="V36" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="W36" s="53" t="s">
+      <c r="W36" s="44" t="s">
         <v>36</v>
       </c>
     </row>
@@ -9607,17 +9571,17 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+    <row r="8" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="33" t="s">
         <v>93</v>
       </c>
     </row>
@@ -11667,6 +11631,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -11924,28 +11909,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{188DA7F5-158B-4F2F-BE68-E8B30B468193}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11962,29 +11951,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>